<commit_message>
update doc on log structure
Définir le format d'écriture des logs
Temps de réalisation : 12h
Temps qu’il reste : 0h

Benjamin GRATADE, Jean-Baptiste ROLAND et Kévin DEFARGE
</commit_message>
<xml_diff>
--- a/Docs/logStruct.xlsx
+++ b/Docs/logStruct.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>version</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>GroupLevel</t>
+  </si>
+  <si>
+    <t>CloseLogTimeUtc</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -666,17 +669,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -714,6 +706,32 @@
         <color indexed="64"/>
       </top>
       <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -722,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -796,52 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -871,74 +844,116 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1224,13 +1239,13 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="1.33203125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="1.33203125" style="36" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.33203125" customWidth="1"/>
@@ -1239,48 +1254,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="66"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="48">
-        <v>2</v>
-      </c>
-      <c r="C2" s="67"/>
+      <c r="B2" s="33">
+        <v>3</v>
+      </c>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="34">
         <v>41387</v>
       </c>
-      <c r="C3" s="67"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="69">
+      <c r="B4" s="40">
         <v>41387</v>
       </c>
-      <c r="C4" s="67"/>
+      <c r="C4" s="38"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="67"/>
-      <c r="D5" s="64" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="52"/>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="67"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
@@ -1289,12 +1304,12 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="67"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>0</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>26</v>
@@ -1311,17 +1326,17 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="67"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="7">
+        <f>B2</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
         <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <f>B2</f>
-        <v>2</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>6</v>
@@ -1338,12 +1353,12 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="67"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>27</v>
@@ -1362,28 +1377,28 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="73">
+        <f>B2</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="43">
         <v>1</v>
       </c>
-      <c r="E10" s="30">
-        <f>B2</f>
-        <v>2</v>
-      </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="57" t="s">
         <v>7</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1391,114 +1406,112 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="74">
+      <c r="A11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="44">
         <v>2</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="39" t="s">
+      <c r="F11" s="54"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="55" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="51" t="s">
+      <c r="I12" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="54" t="s">
+      <c r="K12" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="70"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="46" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="71" t="s">
+      <c r="L13" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="57">
+      <c r="B14" s="64"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="35">
+        <f>B2</f>
         <v>3</v>
       </c>
       <c r="E14" s="14">
-        <f>B2</f>
-        <v>2</v>
-      </c>
-      <c r="F14" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="45" t="s">
+      <c r="K14" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="42" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>0</v>
-      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="52"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -1506,35 +1519,24 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="65">
+      <c r="B16" s="66"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="59">
         <v>0</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="60"/>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="58"/>
+      <c r="D20" s="36"/>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
+  <mergeCells count="21">
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A1:B1"/>
@@ -1544,6 +1546,18 @@
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>